<commit_message>
added remove item functionality
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/order_items.xlsx
+++ b/src/main/resources/xlsx/order_items.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="13">
   <si>
     <t>Order ID</t>
   </si>
@@ -50,7 +50,7 @@
     <t>JE</t>
   </si>
   <si>
-    <t>lmao</t>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -95,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -438,7 +438,7 @@
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -458,7 +458,7 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
@@ -478,7 +478,7 @@
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
@@ -498,6 +498,206 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3.200000047683716</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>